<commit_message>
1. modify PC.scala & ID.scala & Top.scala & Consts.scala to support data hazard analyze l 2. add direct rd_data access in ID stage to avoid ID/MEM & ID/WB data hazard 3. add PC_BUBBLE_REG in PC.scala to avoid ID/EX data hazard 4. modify CPUTest.scala to run more cycles for pipeline structure
</commit_message>
<xml_diff>
--- a/doc/pipeline_analyze.xlsx
+++ b/doc/pipeline_analyze.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060" activeTab="2"/>
+    <workbookView windowWidth="22188" windowHeight="9060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pipeline" sheetId="1" r:id="rId1"/>
     <sheet name="hazard" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="ID-MEM-WB" sheetId="4" r:id="rId3"/>
+    <sheet name="ID-EX" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
   <si>
     <t xml:space="preserve">        时钟周期
 指令序列</t>
@@ -66,7 +66,70 @@
     <t>指令i+4</t>
   </si>
   <si>
+    <t>clock i</t>
+  </si>
+  <si>
     <t>reg</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i-1</t>
+    </r>
+  </si>
+  <si>
+    <t>alu_out</t>
+  </si>
+  <si>
+    <t>BUBBLE</t>
+  </si>
+  <si>
+    <t>clock i+1</t>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i-1</t>
+    </r>
+  </si>
+  <si>
+    <t>rd_data</t>
   </si>
 </sst>
 </file>
@@ -79,18 +142,10 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -104,6 +159,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -252,6 +314,20 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -262,18 +338,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -459,7 +535,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -467,7 +543,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="1">
+    <border>
       <left style="medium">
         <color auto="1"/>
       </left>
@@ -476,12 +552,152 @@
         <color auto="1"/>
       </top>
       <bottom/>
-      <diagonal style="thin">
-        <color auto="1"/>
-      </diagonal>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right/>
@@ -489,6 +705,21 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -497,15 +728,6 @@
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -525,33 +747,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -565,16 +761,9 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
@@ -599,7 +788,9 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -656,71 +847,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -849,7 +985,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -861,34 +997,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -973,131 +1109,158 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1628,7 +1791,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:J6"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1637,154 +1800,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="22">
         <v>1</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="23">
         <v>2</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="23">
         <v>3</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="23">
         <v>4</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="23">
         <v>5</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="23">
         <v>6</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="23">
         <v>7</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="23">
         <v>8</v>
       </c>
-      <c r="J1" s="28">
+      <c r="J1" s="42">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="31"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="31"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="22" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="E4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="22" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="31"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="44" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1809,154 +1972,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="22">
         <v>1</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="23">
         <v>2</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="23">
         <v>3</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="23">
         <v>4</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="23">
         <v>5</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="23">
         <v>6</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="23">
         <v>7</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="23">
         <v>8</v>
       </c>
-      <c r="J1" s="28">
+      <c r="J1" s="42">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="31"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="22" t="s">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="31"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="22" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="22" t="s">
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="31"/>
+      <c r="J5" s="43"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="44" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1969,189 +2132,170 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
   <cols>
     <col min="1" max="1" width="16.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="22">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="23">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D1" s="23">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="23">
         <v>4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="23">
         <v>5</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="24">
         <v>6</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="23">
         <v>7</v>
       </c>
-      <c r="I1" s="4">
+      <c r="I1" s="23">
         <v>8</v>
       </c>
-      <c r="J1" s="28">
+      <c r="J1" s="42">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="30"/>
+      <c r="A3" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
+      <c r="A4" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="G4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="H4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="31"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="22" t="s">
+      <c r="A5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="F5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="G5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="H5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="I5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="31"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="22" t="s">
+      <c r="J5" s="43"/>
+    </row>
+    <row r="6" ht="15.15" spans="1:10">
+      <c r="A6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="G6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="H6" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="I6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="J6" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="31"/>
-    </row>
-    <row r="7" ht="15.15" spans="1:10">
-      <c r="A7" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="32" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A3"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2160,14 +2304,147 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="16384" width="8.88888888888889" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" ht="15.15" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" ht="15.15" spans="1:6">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" ht="15.15"/>
+    <row r="6" ht="15.15" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" ht="15.15" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" ht="15.15" spans="1:6">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
1. add explaination of branch hazard and data hazard analyze
</commit_message>
<xml_diff>
--- a/doc/pipeline_analyze.xlsx
+++ b/doc/pipeline_analyze.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060" activeTab="3"/>
+    <workbookView windowWidth="22188" windowHeight="9060" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="pipeline" sheetId="1" r:id="rId1"/>
-    <sheet name="hazard" sheetId="2" r:id="rId2"/>
+    <sheet name="data_hazard" sheetId="2" r:id="rId2"/>
     <sheet name="ID-MEM-WB" sheetId="4" r:id="rId3"/>
     <sheet name="ID-EX" sheetId="5" r:id="rId4"/>
+    <sheet name="branch_hazard" sheetId="6" r:id="rId5"/>
+    <sheet name="br_hazard_analyze" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="44">
   <si>
     <t xml:space="preserve">        时钟周期
 指令序列</t>
@@ -66,13 +68,252 @@
     <t>指令i+4</t>
   </si>
   <si>
+    <t>clock i-1</t>
+  </si>
+  <si>
+    <t>reg</t>
+  </si>
+  <si>
+    <t>IF logic</t>
+  </si>
+  <si>
+    <t>IF REG</t>
+  </si>
+  <si>
+    <t>ID logic</t>
+  </si>
+  <si>
+    <t>ID REG</t>
+  </si>
+  <si>
+    <t>EX logic</t>
+  </si>
+  <si>
+    <t>EX REG</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MEM </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>logic</t>
+    </r>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i-1
+（EX-&gt;WB）</t>
+    </r>
+  </si>
+  <si>
     <t>clock i</t>
   </si>
   <si>
-    <t>reg</t>
-  </si>
-  <si>
-    <t>data</t>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i
+（WB-&gt;ID）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i-1
+（EX-&gt;WB）</t>
+    </r>
+  </si>
+  <si>
+    <t>clock i+1</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（WB-&gt;ID）</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <t>alu_out</t>
+  </si>
+  <si>
+    <t>BUBBLE</t>
+  </si>
+  <si>
+    <t>clock i+2</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i
+（WB-&gt;ID）</t>
+    </r>
+  </si>
+  <si>
+    <t>rd_data</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+  </si>
+  <si>
+    <t>INSTi</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i-1
+（JMP/BR）</t>
+    </r>
   </si>
   <si>
     <r>
@@ -96,26 +337,32 @@
     <r>
       <rPr>
         <sz val="8"/>
-        <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>i-1</t>
+      <t>i-1
+（JMP/BR）</t>
     </r>
-  </si>
-  <si>
-    <t>alu_out</t>
-  </si>
-  <si>
-    <t>BUBBLE</t>
-  </si>
-  <si>
-    <t>clock i+1</t>
   </si>
   <si>
     <r>
       <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JMP/BR
+</t>
     </r>
     <r>
       <rPr>
@@ -125,11 +372,11 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>i-1</t>
+      <t>flag/taget</t>
     </r>
   </si>
   <si>
-    <t>rd_data</t>
+    <t>target</t>
   </si>
 </sst>
 </file>
@@ -142,16 +389,10 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -165,7 +406,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -316,7 +570,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -328,13 +581,39 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -344,12 +623,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -535,7 +808,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -591,9 +864,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -603,24 +874,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -637,15 +891,6 @@
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -676,9 +921,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color auto="1"/>
@@ -810,15 +1053,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -859,6 +1093,32 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -979,55 +1239,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1042,80 +1299,233 @@
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,142 +1535,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1791,7 +2153,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="A1" sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1800,154 +2162,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="33">
         <v>1</v>
       </c>
-      <c r="C1" s="23">
+      <c r="C1" s="34">
         <v>2</v>
       </c>
-      <c r="D1" s="23">
+      <c r="D1" s="34">
         <v>3</v>
       </c>
-      <c r="E1" s="23">
+      <c r="E1" s="34">
         <v>4</v>
       </c>
-      <c r="F1" s="23">
+      <c r="F1" s="34">
         <v>5</v>
       </c>
-      <c r="G1" s="23">
+      <c r="G1" s="34">
         <v>6</v>
       </c>
-      <c r="H1" s="23">
+      <c r="H1" s="34">
         <v>7</v>
       </c>
-      <c r="I1" s="23">
+      <c r="I1" s="34">
         <v>8</v>
       </c>
-      <c r="J1" s="42">
+      <c r="J1" s="50">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="43"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="43"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="43"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="50" t="s">
+      <c r="F5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="43"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="51" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1963,7 +2325,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:J6"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -1972,154 +2334,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="33">
         <v>1</v>
       </c>
-      <c r="C1" s="23">
+      <c r="C1" s="34">
         <v>2</v>
       </c>
-      <c r="D1" s="23">
+      <c r="D1" s="34">
         <v>3</v>
       </c>
-      <c r="E1" s="23">
+      <c r="E1" s="34">
         <v>4</v>
       </c>
-      <c r="F1" s="23">
+      <c r="F1" s="34">
         <v>5</v>
       </c>
-      <c r="G1" s="23">
+      <c r="G1" s="34">
         <v>6</v>
       </c>
-      <c r="H1" s="23">
+      <c r="H1" s="34">
         <v>7</v>
       </c>
-      <c r="I1" s="23">
+      <c r="I1" s="34">
         <v>8</v>
       </c>
-      <c r="J1" s="42">
+      <c r="J1" s="50">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="43"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="43"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="43"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="43"/>
-    </row>
-    <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="38" t="s">
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="51" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2135,7 +2497,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
@@ -2144,154 +2506,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22">
+      <c r="B1" s="33">
         <v>1</v>
       </c>
-      <c r="C1" s="23">
+      <c r="C1" s="34">
         <v>2</v>
       </c>
-      <c r="D1" s="23">
+      <c r="D1" s="34">
         <v>3</v>
       </c>
-      <c r="E1" s="23">
+      <c r="E1" s="34">
         <v>4</v>
       </c>
-      <c r="F1" s="23">
+      <c r="F1" s="34">
         <v>5</v>
       </c>
-      <c r="G1" s="24">
+      <c r="G1" s="77">
         <v>6</v>
       </c>
-      <c r="H1" s="23">
+      <c r="H1" s="34">
         <v>7</v>
       </c>
-      <c r="I1" s="23">
+      <c r="I1" s="34">
         <v>8</v>
       </c>
-      <c r="J1" s="42">
+      <c r="J1" s="50">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="43"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="43"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="43"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="34" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="G5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="43"/>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="51" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2304,10 +2666,545 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="16384" width="8.88888888888889" style="41"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="54"/>
+    </row>
+    <row r="2" ht="15.15" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="57"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="58"/>
+    </row>
+    <row r="5" ht="15.15" spans="1:8">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" ht="15.15" spans="1:8">
+      <c r="A6" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="54"/>
+    </row>
+    <row r="7" ht="15.15" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="57"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="58"/>
+    </row>
+    <row r="10" ht="15.15" spans="1:8">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" ht="15.15" spans="1:8">
+      <c r="A11" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61"/>
+    </row>
+    <row r="12" ht="15.15" spans="1:8">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="57"/>
+    </row>
+    <row r="14" ht="15.15" spans="1:8">
+      <c r="A14" s="14"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="58"/>
+    </row>
+    <row r="15" ht="15.15" spans="1:8">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" ht="15.15" spans="1:8">
+      <c r="A16" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="66"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="67"/>
+    </row>
+    <row r="17" ht="15.15" spans="1:8">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" ht="15.15" spans="1:8">
+      <c r="A19" s="14"/>
+      <c r="B19" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="74" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="75"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="76"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H18:H19"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="16.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.8" spans="1:10">
+      <c r="A1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34">
+        <v>2</v>
+      </c>
+      <c r="D1" s="34">
+        <v>3</v>
+      </c>
+      <c r="E1" s="34">
+        <v>4</v>
+      </c>
+      <c r="F1" s="34">
+        <v>5</v>
+      </c>
+      <c r="G1" s="34">
+        <v>6</v>
+      </c>
+      <c r="H1" s="34">
+        <v>7</v>
+      </c>
+      <c r="I1" s="34">
+        <v>8</v>
+      </c>
+      <c r="J1" s="50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" ht="15.15" spans="1:10">
+      <c r="A6" s="48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -2330,51 +3227,52 @@
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" ht="15.15" spans="1:6">
-      <c r="A4" s="15"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" ht="15.15"/>
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" ht="15.15" spans="1:6">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
     <row r="6" ht="15.15" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2387,63 +3285,197 @@
         <v>12</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="20"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" ht="15.15"/>
+    <row r="11" ht="15.15" spans="1:6">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" ht="15.15" spans="1:6">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="12" t="s">
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="14"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="29"/>
+    </row>
+    <row r="15" ht="15.15"/>
+    <row r="16" ht="15.15" spans="1:6">
+      <c r="A16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" ht="15.15" spans="1:6">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="14"/>
-    </row>
-    <row r="9" ht="15.15" spans="1:6">
-      <c r="A9" s="15"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="17" t="s">
+      <c r="F17" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="B18" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" ht="15.15" spans="1:6">
+      <c r="A19" s="14"/>
+      <c r="B19" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="24">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A16:F16"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C3:C4"/>
     <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1. add pipeline_advance floder 2. integrate alu/br/csr into EX.scala
</commit_message>
<xml_diff>
--- a/doc/pipeline_analyze.xlsx
+++ b/doc/pipeline_analyze.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060" activeTab="5"/>
+    <workbookView windowWidth="22188" windowHeight="9060" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pipeline" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="46">
   <si>
     <t xml:space="preserve">        时钟周期
 指令序列</t>
@@ -93,6 +93,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">MEM </t>
     </r>
     <r>
@@ -111,6 +118,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -130,6 +144,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -146,6 +167,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -164,6 +191,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -178,6 +211,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -211,6 +250,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -235,6 +281,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -250,6 +303,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -265,6 +325,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -283,6 +349,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -300,7 +373,17 @@
     <t>INSTi</t>
   </si>
   <si>
+    <t>注：标黄表示stall_flag逻辑的输入信号产生位置</t>
+  </si>
+  <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -317,6 +400,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -332,6 +422,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -347,6 +443,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -361,6 +463,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">JMP/BR
 </t>
     </r>
@@ -377,6 +486,9 @@
   </si>
   <si>
     <t>target</t>
+  </si>
+  <si>
+    <t>注：标黄表示jump_flag和br_flag的产生位置</t>
   </si>
 </sst>
 </file>
@@ -570,6 +682,7 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -583,14 +696,13 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF00B050"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B050"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -939,6 +1051,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border diagonalDown="1">
       <left style="medium">
         <color auto="1"/>
@@ -1088,19 +1213,6 @@
         <color auto="1"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -1369,7 +1481,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1406,9 +1518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1422,9 +1531,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1451,9 +1557,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1467,11 +1570,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1484,39 +1587,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1526,16 +1629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1565,18 +1659,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1601,10 +1683,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1613,16 +1695,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2162,154 +2244,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="31">
         <v>1</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="32">
         <v>2</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="32">
         <v>3</v>
       </c>
-      <c r="E1" s="34">
+      <c r="E1" s="32">
         <v>4</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="32">
         <v>5</v>
       </c>
-      <c r="G1" s="34">
+      <c r="G1" s="32">
         <v>6</v>
       </c>
-      <c r="H1" s="34">
+      <c r="H1" s="32">
         <v>7</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="32">
         <v>8</v>
       </c>
-      <c r="J1" s="50">
+      <c r="J1" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="13"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="45" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="49" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="49" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2334,154 +2416,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="31">
         <v>1</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="32">
         <v>2</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="32">
         <v>3</v>
       </c>
-      <c r="E1" s="34">
+      <c r="E1" s="32">
         <v>4</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="32">
         <v>5</v>
       </c>
-      <c r="G1" s="34">
+      <c r="G1" s="32">
         <v>6</v>
       </c>
-      <c r="H1" s="34">
+      <c r="H1" s="32">
         <v>7</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="32">
         <v>8</v>
       </c>
-      <c r="J1" s="50">
+      <c r="J1" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="13"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="45" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="48" t="s">
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" ht="15.15" spans="1:10">
+      <c r="A6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="49" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="84" t="s">
+      <c r="G6" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="49" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2506,154 +2588,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="31">
         <v>1</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="32">
         <v>2</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="32">
         <v>3</v>
       </c>
-      <c r="E1" s="34">
+      <c r="E1" s="32">
         <v>4</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="32">
         <v>5</v>
       </c>
-      <c r="G1" s="77">
+      <c r="G1" s="67">
         <v>6</v>
       </c>
-      <c r="H1" s="34">
+      <c r="H1" s="32">
         <v>7</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="32">
         <v>8</v>
       </c>
-      <c r="J1" s="50">
+      <c r="J1" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="79"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="13"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="45" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="45" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="82" t="s">
+      <c r="F5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="49" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="83" t="s">
+      <c r="G6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="49" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2666,28 +2748,28 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="8.88888888888889" style="41"/>
+    <col min="1" max="16384" width="8.88888888888889" style="39"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:8">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="54"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" ht="15.15" spans="1:8">
       <c r="A2" s="5" t="s">
@@ -2708,10 +2790,10 @@
       <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="55" t="s">
+      <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2724,42 +2806,42 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="57"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="58"/>
+      <c r="H3" s="51"/>
+    </row>
+    <row r="4" ht="15.15" spans="1:8">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="52"/>
     </row>
     <row r="5" ht="15.15" spans="1:8">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" ht="15.15" spans="1:8">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" ht="15.15" spans="1:8">
       <c r="A7" s="5" t="s">
@@ -2780,10 +2862,10 @@
       <c r="F7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2794,26 +2876,26 @@
       <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="12"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="57"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="58"/>
+      <c r="H8" s="51"/>
+    </row>
+    <row r="9" ht="15.15" spans="1:8">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="52"/>
     </row>
     <row r="10" ht="15.15" spans="1:8">
       <c r="A10" s="1"/>
@@ -2822,20 +2904,20 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" ht="15.15" spans="1:8">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="61"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="55"/>
     </row>
     <row r="12" ht="15.15" spans="1:8">
       <c r="A12" s="5" t="s">
@@ -2847,19 +2929,19 @@
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="56" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="55" t="s">
+      <c r="G12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="56" t="s">
+      <c r="H12" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2867,63 +2949,63 @@
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="57" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="57"/>
+      <c r="H13" s="51"/>
     </row>
     <row r="14" ht="15.15" spans="1:8">
-      <c r="A14" s="14"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="28" t="s">
+      <c r="A14" s="13"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="58"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="52"/>
     </row>
     <row r="15" ht="15.15" spans="1:8">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" ht="15.15" spans="1:8">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="67"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" ht="15.15" spans="1:8">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -2938,59 +3020,73 @@
       <c r="F17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="55" t="s">
+      <c r="G17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="56" t="s">
+      <c r="H17" s="50" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="70" t="s">
+      <c r="C18" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="72" t="s">
+      <c r="F18" s="62" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="73" t="s">
+      <c r="H18" s="63" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="1:8">
-      <c r="A19" s="14"/>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="75"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="76"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="66"/>
+    </row>
+    <row r="20" ht="15.15"/>
+    <row r="21" ht="15.15" spans="1:8">
+      <c r="A21" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
@@ -3041,154 +3137,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="31">
         <v>1</v>
       </c>
-      <c r="C1" s="34">
+      <c r="C1" s="32">
         <v>2</v>
       </c>
-      <c r="D1" s="34">
+      <c r="D1" s="32">
         <v>3</v>
       </c>
-      <c r="E1" s="34">
+      <c r="E1" s="32">
         <v>4</v>
       </c>
-      <c r="F1" s="34">
+      <c r="F1" s="32">
         <v>5</v>
       </c>
-      <c r="G1" s="34">
+      <c r="G1" s="32">
         <v>6</v>
       </c>
-      <c r="H1" s="34">
+      <c r="H1" s="32">
         <v>7</v>
       </c>
-      <c r="I1" s="34">
+      <c r="I1" s="32">
         <v>8</v>
       </c>
-      <c r="J1" s="50">
+      <c r="J1" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="13"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="45" t="s">
+      <c r="G3" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="13"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="45" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="G4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="41"/>
-      <c r="J4" s="13"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="46" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="49" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="49" t="s">
+      <c r="G6" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="49" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3201,10 +3297,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -3247,29 +3343,21 @@
         <v>20</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" ht="15.15" spans="1:6">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-    </row>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" ht="15.15" spans="1:6">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" ht="15.15"/>
     <row r="6" ht="15.15" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>22</v>
@@ -3305,24 +3393,24 @@
         <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" ht="15.15" spans="1:6">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" ht="15.15"/>
     <row r="11" ht="15.15" spans="1:6">
@@ -3351,7 +3439,7 @@
       <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="20" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3359,31 +3447,31 @@
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>41</v>
+      <c r="C13" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="14"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28" t="s">
+      <c r="E13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" ht="15.15" spans="1:6">
+      <c r="A14" s="13"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="29"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" ht="15.15"/>
     <row r="16" ht="15.15" spans="1:6">
@@ -3420,7 +3508,7 @@
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -3429,33 +3517,45 @@
       <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="1:6">
-      <c r="A19" s="14"/>
-      <c r="B19" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="28" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="17"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="16"/>
+    </row>
+    <row r="20" ht="15.15"/>
+    <row r="21" ht="15.15" spans="1:6">
+      <c r="A21" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>

</xml_diff>

<commit_message>
1. change src/main/resources/ctest to src/main/resources/ctest/umimp
</commit_message>
<xml_diff>
--- a/doc/pipeline_analyze.xlsx
+++ b/doc/pipeline_analyze.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060" activeTab="3"/>
+    <workbookView windowWidth="22188" windowHeight="9060" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="pipeline" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="ID-EX" sheetId="5" r:id="rId4"/>
     <sheet name="branch_hazard" sheetId="6" r:id="rId5"/>
     <sheet name="br_hazard_analyze" sheetId="7" r:id="rId6"/>
+    <sheet name="branch_prediction" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="57">
   <si>
     <t xml:space="preserve">        时钟周期
 指令序列</t>
@@ -191,12 +192,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -373,7 +368,8 @@
     <t>INSTi</t>
   </si>
   <si>
-    <t>注：标黄表示stall_flag逻辑的输入信号产生位置</t>
+    <t xml:space="preserve">注：标黄表示stall_flag逻辑的输入信号产生位置；受stall_flag影响，相关信号在相应时钟周期被舍弃（红色）并替换为正确信号（绿色）；stall_flag信号在clocki+1时产生（黄色标识），由ID的逻辑部分ID logic和其流水线寄存器ID REG产生。而对于逻辑电路ID logic，stall_flag对ID logic的影响（使其内的insti变为BUBBLE）发生在同一周期，而对于时序电路部分IF logic（含有reg_pc）和IF REG的影响则在下一周期体现。
+</t>
   </si>
   <si>
     <r>
@@ -449,6 +445,26 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -488,7 +504,183 @@
     <t>target</t>
   </si>
   <si>
-    <t>注：标黄表示jump_flag和br_flag的产生位置</t>
+    <t>注：标黄表示jump_flag和br_flag的产生位置；受jump/br_flag/target影响，相关信号在相应时钟周期被舍弃（红色）并替换为正确信号（绿色）</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pred_PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <t>INSTj</t>
+  </si>
+  <si>
+    <t>注：标黄表示jump/br_target和pred_miss信号产生时间；阴影部分表示预测不命中后的更正指令，橙色表示该信号在该周期受pred_miss_flag和br_target/jump_target的作用改变</t>
   </si>
 </sst>
 </file>
@@ -501,7 +693,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +717,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -682,7 +882,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -696,19 +895,28 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFC000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -718,6 +926,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +1140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1056,9 +1276,16 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -1213,6 +1440,19 @@
         <color auto="1"/>
       </right>
       <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -1351,76 +1591,70 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1429,10 +1663,10 @@
     <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1441,10 +1675,10 @@
     <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1453,10 +1687,10 @@
     <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1465,10 +1699,10 @@
     <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1477,24 +1711,30 @@
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1533,12 +1773,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1551,33 +1797,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1590,39 +1881,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1632,7 +1920,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1656,37 +1947,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1695,16 +1989,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2244,154 +2538,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="32">
+      <c r="G1" s="50">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2416,154 +2710,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="32">
+      <c r="G1" s="50">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2588,154 +2882,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="67">
+      <c r="G1" s="85">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2748,28 +3042,28 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="8.88888888888889" style="39"/>
+    <col min="1" max="16384" width="8.88888888888889" style="35"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" ht="15.15" spans="1:8">
       <c r="A2" s="5" t="s">
@@ -2793,7 +3087,7 @@
       <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="67" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2806,10 +3100,10 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="51"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" ht="15.15" spans="1:8">
       <c r="A4" s="13"/>
@@ -2819,29 +3113,29 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="52"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" ht="15.15" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" ht="15.15" spans="1:8">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" ht="15.15" spans="1:8">
       <c r="A7" s="5" t="s">
@@ -2865,7 +3159,7 @@
       <c r="G7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="67" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2876,50 +3170,50 @@
       <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="51"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="9" ht="15.15" spans="1:8">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="15"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="52"/>
+      <c r="H9" s="69"/>
     </row>
     <row r="10" ht="15.15" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" ht="15.15" spans="1:8">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="55"/>
-    </row>
-    <row r="12" ht="15.15" spans="1:8">
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="72"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -2929,10 +3223,10 @@
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="73" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -2941,7 +3235,7 @@
       <c r="G12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="67" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2949,48 +3243,48 @@
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="74" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="51"/>
-    </row>
-    <row r="14" ht="15.15" spans="1:8">
+      <c r="H13" s="68"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="13"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="25" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="19"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="52"/>
-    </row>
-    <row r="15" ht="15.15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H14" s="69"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" ht="15.15" spans="1:8">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="76" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="6"/>
@@ -3005,7 +3299,7 @@
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="76" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -3023,62 +3317,112 @@
       <c r="G17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="67" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="62" t="s">
+      <c r="F18" s="80" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="81" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="1:8">
       <c r="A19" s="13"/>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="66"/>
+      <c r="H19" s="84"/>
     </row>
     <row r="20" ht="15.15"/>
-    <row r="21" ht="15.15" spans="1:8">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="40"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -3086,7 +3430,6 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
@@ -3116,6 +3459,7 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="H18:H19"/>
+    <mergeCell ref="A21:H26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3137,154 +3481,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="32">
+      <c r="G1" s="50">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="44" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3297,26 +3641,26 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="16384" width="8.88888888888889" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" ht="15.15" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -3359,14 +3703,14 @@
     </row>
     <row r="5" ht="15.15"/>
     <row r="6" ht="15.15" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" ht="15.15" spans="1:6">
       <c r="A7" s="5" t="s">
@@ -3395,33 +3739,33 @@
       <c r="B8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" ht="15.15" spans="1:6">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="16"/>
     </row>
     <row r="10" ht="15.15"/>
     <row r="11" ht="15.15" spans="1:6">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" ht="15.15" spans="1:6">
       <c r="A12" s="5" t="s">
@@ -3439,7 +3783,7 @@
       <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3447,42 +3791,42 @@
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>42</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>43</v>
+      <c r="F13" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" ht="15.15" spans="1:6">
       <c r="A14" s="13"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="25" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="26"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" ht="15.15"/>
     <row r="16" ht="15.15" spans="1:6">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" ht="15.15" spans="1:6">
       <c r="A17" s="5" t="s">
@@ -3508,7 +3852,7 @@
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -3517,37 +3861,52 @@
       <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="1:6">
       <c r="A19" s="13"/>
-      <c r="B19" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="25" t="s">
+      <c r="B19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="19"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" ht="15.15"/>
-    <row r="21" ht="15.15" spans="1:6">
-      <c r="A21" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
+    <row r="21" spans="1:6">
+      <c r="A21" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -3555,7 +3914,6 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
@@ -3576,6 +3934,382 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A21:F23"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" ht="15.15" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" ht="15.15" spans="1:8">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" ht="15.15" spans="1:8">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" ht="15.15" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" ht="15.15" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" ht="15.15" spans="1:8">
+      <c r="A9" s="13"/>
+      <c r="B9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" ht="15.15" spans="1:8">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="15.15" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" ht="15.15" spans="1:8">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="15.15" spans="1:8">
+      <c r="A14" s="13"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" ht="15.15" spans="1:8">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" ht="15.15" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" ht="15.15" spans="1:8">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" ht="15.15" spans="1:8">
+      <c r="A19" s="13"/>
+      <c r="B19" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" ht="15.15" spans="1:8">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A21:F23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
1. add branch prediction in class pipeline_advance -1.1 add BP.scala with 2-level branch predictor and BTB -1.2 add pred_miss_flag logic in Stall.scala -1.3 add pc/inst update logic in PC/PC_BUBBLE_REG/ID.scala with pred_miss_flag 2. complete riscv-tests for pipeline_advance -2.1 add prediction hit rate calculation in RiscvTests_temp.scala 3. complete related doc
</commit_message>
<xml_diff>
--- a/doc/pipeline_analyze.xlsx
+++ b/doc/pipeline_analyze.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9060" activeTab="3"/>
+    <workbookView windowWidth="22188" windowHeight="9060" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="pipeline" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="ID-EX" sheetId="5" r:id="rId4"/>
     <sheet name="branch_hazard" sheetId="6" r:id="rId5"/>
     <sheet name="br_hazard_analyze" sheetId="7" r:id="rId6"/>
+    <sheet name="branch_prediction" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="57">
   <si>
     <t xml:space="preserve">        时钟周期
 指令序列</t>
@@ -191,12 +192,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>PC</t>
     </r>
     <r>
@@ -373,7 +368,8 @@
     <t>INSTi</t>
   </si>
   <si>
-    <t>注：标黄表示stall_flag逻辑的输入信号产生位置</t>
+    <t xml:space="preserve">注：标黄表示stall_flag逻辑的输入信号产生位置；受stall_flag影响，相关信号在相应时钟周期被舍弃（红色）并替换为正确信号（绿色）；stall_flag信号在clocki+1时产生（黄色标识），由ID的逻辑部分ID logic和其流水线寄存器ID REG产生。而对于逻辑电路ID logic，stall_flag对ID logic的影响（使其内的insti变为BUBBLE）发生在同一周期，而对于时序电路部分IF logic（含有reg_pc）和IF REG的影响则在下一周期体现。
+</t>
   </si>
   <si>
     <r>
@@ -449,6 +445,26 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>INST</t>
     </r>
     <r>
@@ -488,7 +504,183 @@
     <t>target</t>
   </si>
   <si>
-    <t>注：标黄表示jump_flag和br_flag的产生位置</t>
+    <t>注：标黄表示jump_flag和br_flag的产生位置；受jump/br_flag/target影响，相关信号在相应时钟周期被舍弃（红色）并替换为正确信号（绿色）</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>i</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pred_PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF00B050"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j+1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>INST</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>j</t>
+    </r>
+  </si>
+  <si>
+    <t>INSTj</t>
+  </si>
+  <si>
+    <t>注：标黄表示jump/br_target和pred_miss信号产生时间；阴影部分表示预测不命中后的更正指令，橙色表示该信号在该周期受pred_miss_flag和br_target/jump_target的作用改变</t>
   </si>
 </sst>
 </file>
@@ -501,7 +693,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,6 +717,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -682,7 +882,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -696,19 +895,28 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFC000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -718,6 +926,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.15"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +1140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1056,9 +1276,16 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -1213,6 +1440,19 @@
         <color auto="1"/>
       </right>
       <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="medium">
@@ -1351,76 +1591,70 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1429,10 +1663,10 @@
     <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1441,10 +1675,10 @@
     <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1453,10 +1687,10 @@
     <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1465,10 +1699,10 @@
     <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1477,24 +1711,30 @@
     <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1533,12 +1773,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1551,33 +1797,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1590,39 +1881,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1632,7 +1920,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1656,37 +1947,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1695,16 +1989,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2244,154 +2538,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="32">
+      <c r="G1" s="50">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2416,154 +2710,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="32">
+      <c r="G1" s="50">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2588,154 +2882,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="67">
+      <c r="G1" s="85">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="E2" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="43" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="73" t="s">
+      <c r="G6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2748,28 +3042,28 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="16384" width="8.88888888888889" style="39"/>
+    <col min="1" max="16384" width="8.88888888888889" style="35"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" ht="15.15" spans="1:8">
       <c r="A2" s="5" t="s">
@@ -2793,7 +3087,7 @@
       <c r="G2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="67" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2806,10 +3100,10 @@
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="51"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" ht="15.15" spans="1:8">
       <c r="A4" s="13"/>
@@ -2819,29 +3113,29 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
-      <c r="H4" s="52"/>
+      <c r="H4" s="69"/>
     </row>
     <row r="5" ht="15.15" spans="1:8">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" ht="15.15" spans="1:8">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
     </row>
     <row r="7" ht="15.15" spans="1:8">
       <c r="A7" s="5" t="s">
@@ -2865,7 +3159,7 @@
       <c r="G7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="67" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2876,50 +3170,50 @@
       <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="10"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="51"/>
+      <c r="H8" s="68"/>
     </row>
     <row r="9" ht="15.15" spans="1:8">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="15"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
-      <c r="H9" s="52"/>
+      <c r="H9" s="69"/>
     </row>
     <row r="10" ht="15.15" spans="1:8">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" ht="15.15" spans="1:8">
-      <c r="A11" s="53" t="s">
+      <c r="A11" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="55"/>
-    </row>
-    <row r="12" ht="15.15" spans="1:8">
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="72"/>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
@@ -2929,10 +3223,10 @@
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="56" t="s">
+      <c r="E12" s="73" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="6" t="s">
@@ -2941,7 +3235,7 @@
       <c r="G12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="67" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2949,48 +3243,48 @@
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="74" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="51"/>
-    </row>
-    <row r="14" ht="15.15" spans="1:8">
+      <c r="H13" s="68"/>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="13"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="25" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="19"/>
+      <c r="E14" s="21"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="H14" s="52"/>
-    </row>
-    <row r="15" ht="15.15" spans="1:8">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H14" s="69"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" ht="15.15" spans="1:8">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="76" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="6"/>
@@ -3005,7 +3299,7 @@
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="76" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -3023,62 +3317,112 @@
       <c r="G17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="67" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="62" t="s">
+      <c r="F18" s="80" t="s">
         <v>30</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="63" t="s">
+      <c r="H18" s="81" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="1:8">
       <c r="A19" s="13"/>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="D19" s="83"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="14"/>
-      <c r="H19" s="66"/>
+      <c r="H19" s="84"/>
     </row>
     <row r="20" ht="15.15"/>
-    <row r="21" ht="15.15" spans="1:8">
-      <c r="A21" s="29" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="40"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -3086,7 +3430,6 @@
     <mergeCell ref="A6:H6"/>
     <mergeCell ref="A11:H11"/>
     <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A21:H21"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
@@ -3116,6 +3459,7 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="H18:H19"/>
+    <mergeCell ref="A21:H26"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3137,154 +3481,154 @@
   </cols>
   <sheetData>
     <row r="1" ht="28.8" spans="1:10">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="49">
         <v>1</v>
       </c>
-      <c r="C1" s="32">
+      <c r="C1" s="50">
         <v>2</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="50">
         <v>3</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="50">
         <v>4</v>
       </c>
-      <c r="F1" s="32">
+      <c r="F1" s="50">
         <v>5</v>
       </c>
-      <c r="G1" s="32">
+      <c r="G1" s="50">
         <v>6</v>
       </c>
-      <c r="H1" s="32">
+      <c r="H1" s="50">
         <v>7</v>
       </c>
-      <c r="I1" s="32">
+      <c r="I1" s="50">
         <v>8</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="65">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="41" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="39"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="44" t="s">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="60" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="12"/>
     </row>
     <row r="6" ht="15.15" spans="1:10">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="49" t="s">
+      <c r="J6" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3297,26 +3641,26 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="16384" width="8.88888888888889" style="1"/>
+    <col min="1" max="16384" width="8.88888888888889" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.15" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" ht="15.15" spans="1:6">
       <c r="A2" s="5" t="s">
@@ -3359,14 +3703,14 @@
     </row>
     <row r="5" ht="15.15"/>
     <row r="6" ht="15.15" spans="1:6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" ht="15.15" spans="1:6">
       <c r="A7" s="5" t="s">
@@ -3395,33 +3739,33 @@
       <c r="B8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" ht="15.15" spans="1:6">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
       <c r="F9" s="16"/>
     </row>
     <row r="10" ht="15.15"/>
     <row r="11" ht="15.15" spans="1:6">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" ht="15.15" spans="1:6">
       <c r="A12" s="5" t="s">
@@ -3439,7 +3783,7 @@
       <c r="E12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3447,42 +3791,42 @@
       <c r="A13" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="23" t="s">
         <v>42</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>43</v>
+      <c r="F13" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" ht="15.15" spans="1:6">
       <c r="A14" s="13"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="25" t="s">
+      <c r="B14" s="46"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="26"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="30"/>
     </row>
     <row r="15" ht="15.15"/>
     <row r="16" ht="15.15" spans="1:6">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" ht="15.15" spans="1:6">
       <c r="A17" s="5" t="s">
@@ -3508,7 +3852,7 @@
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -3517,37 +3861,52 @@
       <c r="D18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="1:6">
       <c r="A19" s="13"/>
-      <c r="B19" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="25" t="s">
+      <c r="B19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="19"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" ht="15.15"/>
-    <row r="21" ht="15.15" spans="1:6">
-      <c r="A21" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
+    <row r="21" spans="1:6">
+      <c r="A21" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="25">
@@ -3555,7 +3914,6 @@
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A16:F16"/>
-    <mergeCell ref="A21:F21"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A13:A14"/>
@@ -3576,6 +3934,382 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A21:F23"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
+  <sheetData>
+    <row r="1" ht="15.15" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" ht="15.15" spans="1:8">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" ht="15.15" spans="1:8">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" ht="15.15" spans="1:8">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" ht="15.15" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" ht="15.15" spans="1:8">
+      <c r="A7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" ht="15.15" spans="1:8">
+      <c r="A9" s="13"/>
+      <c r="B9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" ht="15.15" spans="1:8">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" ht="15.15" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" ht="15.15" spans="1:8">
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" ht="15.15" spans="1:8">
+      <c r="A14" s="13"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" ht="15.15" spans="1:8">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" ht="15.15" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" ht="15.15" spans="1:8">
+      <c r="A17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" ht="15.15" spans="1:8">
+      <c r="A19" s="13"/>
+      <c r="B19" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" ht="15.15" spans="1:8">
+      <c r="A20" s="35"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="42"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A21:F23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>